<commit_message>
selenium working with contact form
</commit_message>
<xml_diff>
--- a/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
+++ b/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\World_Cup_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{97F8D0B3-D4FB-4D98-AB10-F633E3C104D7}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{325294D4-ABC0-4ED8-B4A2-1AA405779BE4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="2835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,7 +592,7 @@
       <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>15</v>
@@ -691,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
@@ -711,7 +711,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -739,7 +739,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
@@ -748,10 +748,10 @@
         <v>23</v>
       </c>
       <c r="G5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -767,7 +767,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>25</v>
@@ -776,10 +776,10 @@
         <v>26</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -795,7 +795,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>28</v>
@@ -804,10 +804,10 @@
         <v>29</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -823,7 +823,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>31</v>
@@ -835,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -851,7 +851,7 @@
         <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>34</v>
@@ -860,7 +860,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
WM with correct policy parameter
</commit_message>
<xml_diff>
--- a/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
+++ b/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\World_Cup_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{2D47DCD0-4A15-40FD-84FC-26399B0325FE}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{D2E7CA0F-D69C-4396-B006-5307B7AE69BD}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="2835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,7 +592,7 @@
       <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +963,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>45</v>
@@ -972,7 +972,7 @@
         <v>46</v>
       </c>
       <c r="G13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
@@ -991,7 +991,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>47</v>
@@ -1000,7 +1000,7 @@
         <v>48</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
@@ -1019,7 +1019,7 @@
         <v>49</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>50</v>
@@ -1028,10 +1028,10 @@
         <v>51</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>

</xml_diff>

<commit_message>
WM with 32 table
</commit_message>
<xml_diff>
--- a/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
+++ b/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\World_Cup_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{58257981-BE52-4A71-97D9-D287624CE43E}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{023C2F12-26AE-40A5-AF90-EE4681A892E3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="2835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,7 +592,7 @@
       <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1215,7 @@
         <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>32</v>
@@ -1224,10 +1224,10 @@
         <v>26</v>
       </c>
       <c r="G22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1243,7 +1243,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>25</v>
@@ -1252,7 +1252,7 @@
         <v>31</v>
       </c>
       <c r="G23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
@@ -1271,7 +1271,7 @@
         <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>28</v>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1604,16 +1604,16 @@
         <v>43276.875</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G36" s="2">
         <v>0</v>
@@ -1632,16 +1632,16 @@
         <v>43276.875</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G37" s="2">
         <v>0</v>
@@ -1716,16 +1716,16 @@
         <v>43277.875</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G40" s="2">
         <v>0</v>
@@ -1744,16 +1744,16 @@
         <v>43277.875</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G41" s="2">
         <v>0</v>
@@ -1884,16 +1884,16 @@
         <v>43279.708333333343</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G46" s="2">
         <v>0</v>
@@ -1912,16 +1912,16 @@
         <v>43279.708333333343</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G47" s="2">
         <v>0</v>
@@ -1940,16 +1940,16 @@
         <v>43279.875</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G48" s="2">
         <v>0</v>
@@ -1968,16 +1968,16 @@
         <v>43279.875</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G49" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
problem with last test match solved
</commit_message>
<xml_diff>
--- a/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
+++ b/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\World_Cup_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{5AEFA544-57D1-45BE-9880-87DB9779DBC1}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{5EB0A01D-1572-4642-806C-1F3850650528}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="2835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -592,7 +592,7 @@
       <pane xSplit="10" ySplit="1" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,7 +1663,7 @@
         <v>10</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>32</v>
@@ -1691,7 +1691,7 @@
         <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>26</v>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -1719,7 +1719,7 @@
         <v>41</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>29</v>
@@ -1728,10 +1728,10 @@
         <v>34</v>
       </c>
       <c r="G40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -1747,7 +1747,7 @@
         <v>17</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>35</v>
@@ -1756,10 +1756,10 @@
         <v>28</v>
       </c>
       <c r="G41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -1775,7 +1775,7 @@
         <v>14</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>40</v>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -1803,7 +1803,7 @@
         <v>24</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>46</v>
@@ -1812,7 +1812,7 @@
         <v>39</v>
       </c>
       <c r="G43" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
@@ -1831,7 +1831,7 @@
         <v>27</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>38</v>
@@ -1843,7 +1843,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -1859,7 +1859,7 @@
         <v>44</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>43</v>
@@ -1868,10 +1868,10 @@
         <v>37</v>
       </c>
       <c r="G45" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H45" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>

</xml_diff>

<commit_message>
debugger and some corrections for constraints
</commit_message>
<xml_diff>
--- a/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
+++ b/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\World_Cup_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{5EB0A01D-1572-4642-806C-1F3850650528}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{26D1B78A-6790-4B3E-BBAF-0173C65E80A3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="2835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="59">
   <si>
     <t>match_number</t>
   </si>
@@ -589,10 +589,10 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="K26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
+      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,7 +1887,7 @@
         <v>36</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>55</v>
@@ -1899,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="H46" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -1915,7 +1915,7 @@
         <v>49</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>53</v>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="H47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -1943,7 +1943,7 @@
         <v>33</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>51</v>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="H48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -1971,7 +1971,7 @@
         <v>30</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>48</v>
@@ -1980,10 +1980,10 @@
         <v>50</v>
       </c>
       <c r="G49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2001,8 +2001,12 @@
       <c r="D50" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="G50" s="2">
         <v>0</v>
       </c>
@@ -2025,8 +2029,12 @@
       <c r="D51" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G51" s="2">
         <v>0</v>
       </c>
@@ -2049,8 +2057,12 @@
       <c r="D52" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G52" s="2">
         <v>0</v>
       </c>
@@ -2073,8 +2085,12 @@
       <c r="D53" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
+      <c r="E53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G53" s="2">
         <v>0</v>
       </c>
@@ -2097,8 +2113,12 @@
       <c r="D54" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
+      <c r="E54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G54" s="2">
         <v>0</v>
       </c>
@@ -2121,8 +2141,12 @@
       <c r="D55" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G55" s="2">
         <v>0</v>
       </c>
@@ -2145,8 +2169,12 @@
       <c r="D56" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="G56" s="2">
         <v>0</v>
       </c>
@@ -2169,8 +2197,12 @@
       <c r="D57" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="G57" s="2">
         <v>0</v>
       </c>
@@ -2374,7 +2406,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fibonacci with some more checks
</commit_message>
<xml_diff>
--- a/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
+++ b/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\World_Cup_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{26D1B78A-6790-4B3E-BBAF-0173C65E80A3}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{E527E8C2-36F4-4F43-931F-75EE4AC3FBFD}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="2835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="59">
   <si>
     <t>match_number</t>
   </si>
@@ -589,10 +589,10 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="K38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomRight" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,7 +1999,7 @@
         <v>24</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>25</v>
@@ -2008,10 +2008,10 @@
         <v>28</v>
       </c>
       <c r="G50" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H50" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2027,7 +2027,7 @@
         <v>21</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>16</v>
@@ -2036,10 +2036,10 @@
         <v>22</v>
       </c>
       <c r="G51" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2055,7 +2055,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>23</v>
@@ -2064,10 +2064,10 @@
         <v>12</v>
       </c>
       <c r="G52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2083,7 +2083,7 @@
         <v>44</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>34</v>
@@ -2092,10 +2092,10 @@
         <v>32</v>
       </c>
       <c r="G53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2111,7 +2111,7 @@
         <v>36</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>42</v>
@@ -2120,7 +2120,7 @@
         <v>40</v>
       </c>
       <c r="G54" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H54" s="2">
         <v>0</v>
@@ -2139,7 +2139,7 @@
         <v>41</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>47</v>
@@ -2148,10 +2148,10 @@
         <v>53</v>
       </c>
       <c r="G55" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -2167,7 +2167,7 @@
         <v>17</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>45</v>
@@ -2176,7 +2176,7 @@
         <v>43</v>
       </c>
       <c r="G56" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" s="2">
         <v>0</v>
@@ -2195,7 +2195,7 @@
         <v>27</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>52</v>
@@ -2204,10 +2204,10 @@
         <v>51</v>
       </c>
       <c r="G57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -2225,8 +2225,12 @@
       <c r="D58" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G58" s="2">
         <v>0</v>
       </c>
@@ -2249,8 +2253,12 @@
       <c r="D59" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G59" s="2">
         <v>0</v>
       </c>
@@ -2273,8 +2281,12 @@
       <c r="D60" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="E60" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="G60" s="2">
         <v>0</v>
       </c>
@@ -2297,8 +2309,12 @@
       <c r="D61" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G61" s="2">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Crypto currencies - load and detection
</commit_message>
<xml_diff>
--- a/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
+++ b/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\World_Cup_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{E527E8C2-36F4-4F43-931F-75EE4AC3FBFD}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{F8022EA5-E371-4E2E-838C-5C7E549795C8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="2835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="59">
   <si>
     <t>match_number</t>
   </si>
@@ -592,7 +592,7 @@
       <pane xSplit="10" ySplit="1" topLeftCell="K38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomRight" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2223,7 +2223,7 @@
         <v>44</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>25</v>
@@ -2232,7 +2232,7 @@
         <v>16</v>
       </c>
       <c r="G58" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H58" s="2">
         <v>0</v>
@@ -2251,7 +2251,7 @@
         <v>24</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>47</v>
@@ -2260,10 +2260,10 @@
         <v>42</v>
       </c>
       <c r="G59" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H59" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -2279,7 +2279,7 @@
         <v>36</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>51</v>
@@ -2288,7 +2288,7 @@
         <v>45</v>
       </c>
       <c r="G60" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H60" s="2">
         <v>0</v>
@@ -2307,7 +2307,7 @@
         <v>21</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>12</v>
@@ -2316,10 +2316,10 @@
         <v>34</v>
       </c>
       <c r="G61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -2337,8 +2337,12 @@
       <c r="D62" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="G62" s="2">
         <v>0</v>
       </c>
@@ -2361,8 +2365,12 @@
       <c r="D63" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="G63" s="2">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Problems with longer crypto keys (like DOGE, BAND) solved.
</commit_message>
<xml_diff>
--- a/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
+++ b/Gaming/World_Cup_2018/Fifa_world_cup_2018_matches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\OneDrive\GitHub\PycharmProjects\Gaming\World_Cup_2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b7b412bfd75d269/GitHub/PycharmProjects/Gaming/World_Cup_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{B5894BB7-8DE1-4B98-B6DD-0B0879B2B084}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="11_B8C29A7985D4435D6CEA363750C3B65254F40870" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E47BC817-31FA-43A2-912A-48C5506A0CB7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="2835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21015" yWindow="180" windowWidth="13935" windowHeight="19245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fifa_world_cup_2018_matches" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -589,13 +589,13 @@
   <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="1" topLeftCell="K38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="1" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F64" sqref="F64"/>
+      <selection pane="bottomRight" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
@@ -2363,7 +2363,7 @@
         <v>10</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>34</v>
@@ -2400,7 +2400,7 @@
         <v>51</v>
       </c>
       <c r="G64" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H64" s="2">
         <v>0</v>
@@ -2428,10 +2428,10 @@
         <v>34</v>
       </c>
       <c r="G65" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H65" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
@@ -2453,7 +2453,7 @@
       <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>

</xml_diff>